<commit_message>
Add, Update and Delete for Eduction in profile
</commit_message>
<xml_diff>
--- a/MarsQA-1/SpecflowTests/Data/Data.xlsx
+++ b/MarsQA-1/SpecflowTests/Data/Data.xlsx
@@ -9,7 +9,8 @@
   </bookViews>
   <sheets>
     <sheet name="Language" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Skill" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Education" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Skill" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t xml:space="preserve">Language</t>
   </si>
@@ -39,6 +40,45 @@
   </si>
   <si>
     <t xml:space="preserve">Native/Bilingual </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CollegeName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YearOfPassing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BHU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M.A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archeology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.Tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrical</t>
   </si>
   <si>
     <t xml:space="preserve">Skill</t>
@@ -131,7 +171,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -142,6 +182,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -227,9 +271,89 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.33"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>2011</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -240,7 +364,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -248,15 +372,15 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B2" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>2</v>

</xml_diff>